<commit_message>
updated sales sheet name, and started with jp notebooks
</commit_message>
<xml_diff>
--- a/SALES LOG - XYZ COMPANY.xlsx
+++ b/SALES LOG - XYZ COMPANY.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmfon\Documents\Automation_Project\First-automation-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{51E74235-CA84-4BA2-9EE2-BF60BA805215}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51BD0FB3-AC7B-4EE6-A161-6050B735414B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="699" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="9 - MAR 2020" sheetId="20" r:id="rId1"/>
+    <sheet name="daily_totals" sheetId="20" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'9 - MAR 2020'!$A$1:$Y$178</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'9 - MAR 2020'!$A$1:$U$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">daily_totals!$A$1:$Y$178</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">daily_totals!$A$1:$U$1</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -229,7 +229,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="m/d/yy;@"/>
-    <numFmt numFmtId="167" formatCode="mm/dd/yy;@"/>
+    <numFmt numFmtId="166" formatCode="mm/dd/yy;@"/>
   </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
@@ -609,7 +609,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -618,7 +618,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -627,7 +627,7 @@
     <xf numFmtId="164" fontId="9" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="9" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="9" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -639,7 +639,7 @@
     <xf numFmtId="165" fontId="3" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="3" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="43" fontId="3" fillId="3" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -673,7 +673,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="3" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="3" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -740,16 +740,16 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="44" fontId="3" fillId="3" borderId="15" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="10" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="10" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="10" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="10" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1045,8 +1045,8 @@
   </sheetPr>
   <dimension ref="A1:AI187"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="T1" sqref="T1"/>
     </sheetView>
   </sheetViews>
@@ -9123,10 +9123,10 @@
         <f>$F$160</f>
         <v>43910</v>
       </c>
-      <c r="G162" s="69" t="s">
+      <c r="G162" s="70" t="s">
         <v>4</v>
       </c>
-      <c r="H162" s="69"/>
+      <c r="H162" s="70"/>
       <c r="I162" s="37"/>
       <c r="J162" s="48"/>
       <c r="K162" s="46" t="s">
@@ -9184,8 +9184,8 @@
         <f t="shared" ref="F164:F174" si="3">$F$160</f>
         <v>43910</v>
       </c>
-      <c r="G164" s="70"/>
-      <c r="H164" s="70"/>
+      <c r="G164" s="69"/>
+      <c r="H164" s="69"/>
       <c r="I164" s="52"/>
       <c r="J164" s="48"/>
       <c r="K164" s="50" t="s">
@@ -9229,8 +9229,8 @@
         <f t="shared" si="3"/>
         <v>43910</v>
       </c>
-      <c r="G165" s="70"/>
-      <c r="H165" s="70"/>
+      <c r="G165" s="69"/>
+      <c r="H165" s="69"/>
       <c r="I165" s="52"/>
       <c r="J165" s="48"/>
       <c r="K165" s="26"/>
@@ -9269,8 +9269,8 @@
         <f t="shared" si="3"/>
         <v>43910</v>
       </c>
-      <c r="G166" s="70"/>
-      <c r="H166" s="70"/>
+      <c r="G166" s="69"/>
+      <c r="H166" s="69"/>
       <c r="I166" s="52"/>
       <c r="J166" s="48"/>
       <c r="K166" s="59" t="s">
@@ -9311,10 +9311,10 @@
         <f t="shared" si="3"/>
         <v>43910</v>
       </c>
-      <c r="G167" s="70" t="s">
+      <c r="G167" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="H167" s="70"/>
+      <c r="H167" s="69"/>
       <c r="I167" s="52"/>
       <c r="J167" s="48"/>
       <c r="K167" s="61" t="s">
@@ -9358,8 +9358,8 @@
         <f t="shared" si="3"/>
         <v>43910</v>
       </c>
-      <c r="G168" s="70"/>
-      <c r="H168" s="70"/>
+      <c r="G168" s="69"/>
+      <c r="H168" s="69"/>
       <c r="I168" s="52"/>
       <c r="J168" s="48"/>
       <c r="K168" s="61" t="s">
@@ -9403,8 +9403,8 @@
         <f t="shared" si="3"/>
         <v>43910</v>
       </c>
-      <c r="G169" s="70"/>
-      <c r="H169" s="70"/>
+      <c r="G169" s="69"/>
+      <c r="H169" s="69"/>
       <c r="I169" s="52"/>
       <c r="J169" s="48"/>
       <c r="K169" s="61" t="s">
@@ -9448,8 +9448,8 @@
         <f t="shared" si="3"/>
         <v>43910</v>
       </c>
-      <c r="G170" s="70"/>
-      <c r="H170" s="70"/>
+      <c r="G170" s="69"/>
+      <c r="H170" s="69"/>
       <c r="I170" s="52"/>
       <c r="J170" s="48"/>
       <c r="K170" s="61" t="s">
@@ -9493,8 +9493,8 @@
         <f t="shared" si="3"/>
         <v>43910</v>
       </c>
-      <c r="G171" s="70"/>
-      <c r="H171" s="70"/>
+      <c r="G171" s="69"/>
+      <c r="H171" s="69"/>
       <c r="I171" s="52"/>
       <c r="J171" s="48"/>
       <c r="K171" s="61" t="s">
@@ -9538,8 +9538,8 @@
         <f t="shared" si="3"/>
         <v>43910</v>
       </c>
-      <c r="G172" s="70"/>
-      <c r="H172" s="70"/>
+      <c r="G172" s="69"/>
+      <c r="H172" s="69"/>
       <c r="I172" s="52"/>
       <c r="J172" s="48"/>
       <c r="K172" s="61" t="s">
@@ -9583,8 +9583,8 @@
         <f t="shared" si="3"/>
         <v>43910</v>
       </c>
-      <c r="G173" s="70"/>
-      <c r="H173" s="70"/>
+      <c r="G173" s="69"/>
+      <c r="H173" s="69"/>
       <c r="I173" s="52"/>
       <c r="J173" s="48"/>
       <c r="K173" s="61" t="s">
@@ -9972,18 +9972,18 @@
   </sheetData>
   <autoFilter ref="A1:Y178" xr:uid="{00000000-0009-0000-0000-000009000000}"/>
   <mergeCells count="12">
+    <mergeCell ref="G162:H162"/>
+    <mergeCell ref="G165:H165"/>
+    <mergeCell ref="G166:H166"/>
+    <mergeCell ref="G167:H167"/>
+    <mergeCell ref="A164:B164"/>
+    <mergeCell ref="G164:H164"/>
     <mergeCell ref="G173:H173"/>
     <mergeCell ref="G168:H168"/>
     <mergeCell ref="G169:H169"/>
     <mergeCell ref="G170:H170"/>
     <mergeCell ref="G171:H171"/>
     <mergeCell ref="G172:H172"/>
-    <mergeCell ref="G162:H162"/>
-    <mergeCell ref="G165:H165"/>
-    <mergeCell ref="G166:H166"/>
-    <mergeCell ref="G167:H167"/>
-    <mergeCell ref="A164:B164"/>
-    <mergeCell ref="G164:H164"/>
   </mergeCells>
   <printOptions horizontalCentered="1" gridLines="1"/>
   <pageMargins left="0" right="0" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9992,66 +9992,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Templates xmlns="665d2a2a-3cfa-45cf-86df-1198654f14e4" xsi:nil="true"/>
-    <Self_Registration_Enabled xmlns="665d2a2a-3cfa-45cf-86df-1198654f14e4" xsi:nil="true"/>
-    <Has_Leaders_Only_SectionGroup xmlns="665d2a2a-3cfa-45cf-86df-1198654f14e4" xsi:nil="true"/>
-    <Is_Collaboration_Space_Locked xmlns="665d2a2a-3cfa-45cf-86df-1198654f14e4" xsi:nil="true"/>
-    <Member_Groups xmlns="665d2a2a-3cfa-45cf-86df-1198654f14e4">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Member_Groups>
-    <CultureName xmlns="665d2a2a-3cfa-45cf-86df-1198654f14e4" xsi:nil="true"/>
-    <DefaultSectionNames xmlns="665d2a2a-3cfa-45cf-86df-1198654f14e4" xsi:nil="true"/>
-    <Invited_Members xmlns="665d2a2a-3cfa-45cf-86df-1198654f14e4" xsi:nil="true"/>
-    <Members xmlns="665d2a2a-3cfa-45cf-86df-1198654f14e4">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Members>
-    <FolderType xmlns="665d2a2a-3cfa-45cf-86df-1198654f14e4" xsi:nil="true"/>
-    <Distribution_Groups xmlns="665d2a2a-3cfa-45cf-86df-1198654f14e4" xsi:nil="true"/>
-    <AppVersion xmlns="665d2a2a-3cfa-45cf-86df-1198654f14e4" xsi:nil="true"/>
-    <LMS_Mappings xmlns="665d2a2a-3cfa-45cf-86df-1198654f14e4" xsi:nil="true"/>
-    <Math_Settings xmlns="665d2a2a-3cfa-45cf-86df-1198654f14e4" xsi:nil="true"/>
-    <Owner xmlns="665d2a2a-3cfa-45cf-86df-1198654f14e4">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Owner>
-    <Invited_Leaders xmlns="665d2a2a-3cfa-45cf-86df-1198654f14e4" xsi:nil="true"/>
-    <IsNotebookLocked xmlns="665d2a2a-3cfa-45cf-86df-1198654f14e4" xsi:nil="true"/>
-    <NotebookType xmlns="665d2a2a-3cfa-45cf-86df-1198654f14e4" xsi:nil="true"/>
-    <Leaders xmlns="665d2a2a-3cfa-45cf-86df-1198654f14e4">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Leaders>
-    <TeamsChannelId xmlns="665d2a2a-3cfa-45cf-86df-1198654f14e4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010085FED89D34111B49913BBC7FDE578531" ma:contentTypeVersion="22" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a506f0c38746fd7cfe988c19abb6dd83">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="665d2a2a-3cfa-45cf-86df-1198654f14e4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="608b8493204b4e817bcdea6cb384484a" ns2:_="">
     <xsd:import namespace="665d2a2a-3cfa-45cf-86df-1198654f14e4"/>
@@ -10371,31 +10311,67 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FBE75A51-F7E8-4D0C-B4A3-87B85271C615}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Templates xmlns="665d2a2a-3cfa-45cf-86df-1198654f14e4" xsi:nil="true"/>
+    <Self_Registration_Enabled xmlns="665d2a2a-3cfa-45cf-86df-1198654f14e4" xsi:nil="true"/>
+    <Has_Leaders_Only_SectionGroup xmlns="665d2a2a-3cfa-45cf-86df-1198654f14e4" xsi:nil="true"/>
+    <Is_Collaboration_Space_Locked xmlns="665d2a2a-3cfa-45cf-86df-1198654f14e4" xsi:nil="true"/>
+    <Member_Groups xmlns="665d2a2a-3cfa-45cf-86df-1198654f14e4">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Member_Groups>
+    <CultureName xmlns="665d2a2a-3cfa-45cf-86df-1198654f14e4" xsi:nil="true"/>
+    <DefaultSectionNames xmlns="665d2a2a-3cfa-45cf-86df-1198654f14e4" xsi:nil="true"/>
+    <Invited_Members xmlns="665d2a2a-3cfa-45cf-86df-1198654f14e4" xsi:nil="true"/>
+    <Members xmlns="665d2a2a-3cfa-45cf-86df-1198654f14e4">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Members>
+    <FolderType xmlns="665d2a2a-3cfa-45cf-86df-1198654f14e4" xsi:nil="true"/>
+    <Distribution_Groups xmlns="665d2a2a-3cfa-45cf-86df-1198654f14e4" xsi:nil="true"/>
+    <AppVersion xmlns="665d2a2a-3cfa-45cf-86df-1198654f14e4" xsi:nil="true"/>
+    <LMS_Mappings xmlns="665d2a2a-3cfa-45cf-86df-1198654f14e4" xsi:nil="true"/>
+    <Math_Settings xmlns="665d2a2a-3cfa-45cf-86df-1198654f14e4" xsi:nil="true"/>
+    <Owner xmlns="665d2a2a-3cfa-45cf-86df-1198654f14e4">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Owner>
+    <Invited_Leaders xmlns="665d2a2a-3cfa-45cf-86df-1198654f14e4" xsi:nil="true"/>
+    <IsNotebookLocked xmlns="665d2a2a-3cfa-45cf-86df-1198654f14e4" xsi:nil="true"/>
+    <NotebookType xmlns="665d2a2a-3cfa-45cf-86df-1198654f14e4" xsi:nil="true"/>
+    <Leaders xmlns="665d2a2a-3cfa-45cf-86df-1198654f14e4">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Leaders>
+    <TeamsChannelId xmlns="665d2a2a-3cfa-45cf-86df-1198654f14e4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{415CDD9D-29A7-491B-BE42-201A411A3D42}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="665d2a2a-3cfa-45cf-86df-1198654f14e4"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9D759083-9B8C-451D-90DE-1D943E2E4B02}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10411,4 +10387,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{415CDD9D-29A7-491B-BE42-201A411A3D42}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="665d2a2a-3cfa-45cf-86df-1198654f14e4"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FBE75A51-F7E8-4D0C-B4A3-87B85271C615}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
updated dataset including using tabula for end report
</commit_message>
<xml_diff>
--- a/SALES LOG - XYZ COMPANY.xlsx
+++ b/SALES LOG - XYZ COMPANY.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmfon\Documents\Automation_Project\First-automation-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51BD0FB3-AC7B-4EE6-A161-6050B735414B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A81609A8-B66A-4ACF-AC86-E51ED7B69E97}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="699" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1040,14 +1040,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB6665E2-1C70-490B-918E-22851D278B7A}">
-  <sheetPr>
+  <sheetPr filterMode="1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:AI187"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T1" sqref="T1"/>
+      <selection pane="bottomLeft" activeCell="E149" sqref="E149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1157,7 +1157,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" s="18">
         <v>1</v>
       </c>
@@ -1207,7 +1207,7 @@
       <c r="X2" s="21"/>
       <c r="Y2" s="21"/>
     </row>
-    <row r="3" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="18">
         <v>1</v>
       </c>
@@ -1257,7 +1257,7 @@
       <c r="X3" s="21"/>
       <c r="Y3" s="21"/>
     </row>
-    <row r="4" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" s="18">
         <v>1</v>
       </c>
@@ -1307,7 +1307,7 @@
       <c r="X4" s="21"/>
       <c r="Y4" s="21"/>
     </row>
-    <row r="5" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" s="18">
         <v>4</v>
       </c>
@@ -1357,7 +1357,7 @@
       <c r="X5" s="21"/>
       <c r="Y5" s="21"/>
     </row>
-    <row r="6" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="18">
         <v>4</v>
       </c>
@@ -1407,7 +1407,7 @@
       <c r="X6" s="21"/>
       <c r="Y6" s="21"/>
     </row>
-    <row r="7" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="18"/>
       <c r="B7" s="19" t="s">
         <v>6</v>
@@ -1455,7 +1455,7 @@
       <c r="X7" s="21"/>
       <c r="Y7" s="21"/>
     </row>
-    <row r="8" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="18">
         <v>4</v>
       </c>
@@ -1505,7 +1505,7 @@
       <c r="X8" s="21"/>
       <c r="Y8" s="21"/>
     </row>
-    <row r="9" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="18">
         <v>2</v>
       </c>
@@ -1559,7 +1559,7 @@
       </c>
       <c r="Y9" s="21"/>
     </row>
-    <row r="10" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="18">
         <v>4</v>
       </c>
@@ -1609,7 +1609,7 @@
       <c r="X10" s="21"/>
       <c r="Y10" s="21"/>
     </row>
-    <row r="11" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="18">
         <v>1</v>
       </c>
@@ -1659,7 +1659,7 @@
       <c r="X11" s="21"/>
       <c r="Y11" s="21"/>
     </row>
-    <row r="12" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="18">
         <v>1</v>
       </c>
@@ -1709,7 +1709,7 @@
       <c r="X12" s="21"/>
       <c r="Y12" s="21"/>
     </row>
-    <row r="13" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="18">
         <v>1</v>
       </c>
@@ -1759,7 +1759,7 @@
       <c r="X13" s="21"/>
       <c r="Y13" s="21"/>
     </row>
-    <row r="14" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="18">
         <v>1</v>
       </c>
@@ -1809,7 +1809,7 @@
       <c r="X14" s="21"/>
       <c r="Y14" s="21"/>
     </row>
-    <row r="15" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="18">
         <v>1</v>
       </c>
@@ -1859,7 +1859,7 @@
       <c r="X15" s="21"/>
       <c r="Y15" s="21"/>
     </row>
-    <row r="16" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="18">
         <v>1</v>
       </c>
@@ -1909,7 +1909,7 @@
       <c r="X16" s="21"/>
       <c r="Y16" s="21"/>
     </row>
-    <row r="17" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="18">
         <v>1</v>
       </c>
@@ -1959,7 +1959,7 @@
       <c r="X17" s="21"/>
       <c r="Y17" s="21"/>
     </row>
-    <row r="18" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="18">
         <v>1</v>
       </c>
@@ -2011,7 +2011,7 @@
       <c r="X18" s="21"/>
       <c r="Y18" s="21"/>
     </row>
-    <row r="19" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="18">
         <v>1</v>
       </c>
@@ -2061,7 +2061,7 @@
       <c r="X19" s="21"/>
       <c r="Y19" s="21"/>
     </row>
-    <row r="20" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="18">
         <v>4</v>
       </c>
@@ -2111,7 +2111,7 @@
       <c r="X20" s="21"/>
       <c r="Y20" s="21"/>
     </row>
-    <row r="21" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="18">
         <v>4</v>
       </c>
@@ -2161,7 +2161,7 @@
       <c r="X21" s="21"/>
       <c r="Y21" s="21"/>
     </row>
-    <row r="22" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="18">
         <v>4</v>
       </c>
@@ -2213,7 +2213,7 @@
         <v>542.44000000000005</v>
       </c>
     </row>
-    <row r="23" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="18">
         <v>3</v>
       </c>
@@ -2263,7 +2263,7 @@
       <c r="X23" s="21"/>
       <c r="Y23" s="21"/>
     </row>
-    <row r="24" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="18">
         <v>3</v>
       </c>
@@ -2313,7 +2313,7 @@
       <c r="X24" s="21"/>
       <c r="Y24" s="21"/>
     </row>
-    <row r="25" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="18">
         <v>1</v>
       </c>
@@ -2363,7 +2363,7 @@
       <c r="X25" s="21"/>
       <c r="Y25" s="21"/>
     </row>
-    <row r="26" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="18">
         <v>1</v>
       </c>
@@ -2413,7 +2413,7 @@
       <c r="X26" s="21"/>
       <c r="Y26" s="21"/>
     </row>
-    <row r="27" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="18">
         <v>1</v>
       </c>
@@ -2463,7 +2463,7 @@
       <c r="X27" s="21"/>
       <c r="Y27" s="21"/>
     </row>
-    <row r="28" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="18">
         <v>1</v>
       </c>
@@ -2513,7 +2513,7 @@
       <c r="X28" s="21"/>
       <c r="Y28" s="21"/>
     </row>
-    <row r="29" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="18">
         <v>4</v>
       </c>
@@ -2565,7 +2565,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" s="18">
         <v>4</v>
       </c>
@@ -2615,7 +2615,7 @@
       <c r="X30" s="21"/>
       <c r="Y30" s="21"/>
     </row>
-    <row r="31" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" s="18">
         <v>4</v>
       </c>
@@ -2663,7 +2663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" s="18">
         <v>1</v>
       </c>
@@ -2713,7 +2713,7 @@
       <c r="X32" s="21"/>
       <c r="Y32" s="21"/>
     </row>
-    <row r="33" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" s="18">
         <v>1</v>
       </c>
@@ -2763,7 +2763,7 @@
       <c r="X33" s="21"/>
       <c r="Y33" s="21"/>
     </row>
-    <row r="34" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" s="18">
         <v>1</v>
       </c>
@@ -2817,7 +2817,7 @@
       <c r="X34" s="21"/>
       <c r="Y34" s="21"/>
     </row>
-    <row r="35" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" s="18">
         <v>1</v>
       </c>
@@ -2867,7 +2867,7 @@
       <c r="X35" s="21"/>
       <c r="Y35" s="21"/>
     </row>
-    <row r="36" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="18">
         <v>1</v>
       </c>
@@ -2917,7 +2917,7 @@
       <c r="X36" s="21"/>
       <c r="Y36" s="21"/>
     </row>
-    <row r="37" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" s="18">
         <v>1</v>
       </c>
@@ -2967,7 +2967,7 @@
       <c r="X37" s="21"/>
       <c r="Y37" s="21"/>
     </row>
-    <row r="38" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" s="18">
         <v>1</v>
       </c>
@@ -3019,7 +3019,7 @@
       <c r="X38" s="21"/>
       <c r="Y38" s="21"/>
     </row>
-    <row r="39" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" s="18">
         <v>5</v>
       </c>
@@ -3071,7 +3071,7 @@
       <c r="X39" s="21"/>
       <c r="Y39" s="21"/>
     </row>
-    <row r="40" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" s="18">
         <v>4</v>
       </c>
@@ -3121,7 +3121,7 @@
       <c r="X40" s="21"/>
       <c r="Y40" s="21"/>
     </row>
-    <row r="41" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" s="18">
         <v>3</v>
       </c>
@@ -3171,7 +3171,7 @@
       <c r="X41" s="21"/>
       <c r="Y41" s="21"/>
     </row>
-    <row r="42" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" s="18">
         <v>3</v>
       </c>
@@ -3257,7 +3257,7 @@
       <c r="X43" s="21"/>
       <c r="Y43" s="21"/>
     </row>
-    <row r="44" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" s="18">
         <v>4</v>
       </c>
@@ -3305,7 +3305,7 @@
       <c r="X44" s="21"/>
       <c r="Y44" s="21"/>
     </row>
-    <row r="45" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" s="18">
         <v>1</v>
       </c>
@@ -3355,7 +3355,7 @@
       <c r="X45" s="21"/>
       <c r="Y45" s="21"/>
     </row>
-    <row r="46" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" s="18">
         <v>1</v>
       </c>
@@ -3405,7 +3405,7 @@
       <c r="X46" s="21"/>
       <c r="Y46" s="21"/>
     </row>
-    <row r="47" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" s="18">
         <v>1</v>
       </c>
@@ -3457,7 +3457,7 @@
       <c r="X47" s="21"/>
       <c r="Y47" s="21"/>
     </row>
-    <row r="48" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" s="18">
         <v>4</v>
       </c>
@@ -3507,7 +3507,7 @@
       <c r="X48" s="21"/>
       <c r="Y48" s="21"/>
     </row>
-    <row r="49" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" s="18">
         <v>1</v>
       </c>
@@ -3559,7 +3559,7 @@
       <c r="X49" s="21"/>
       <c r="Y49" s="21"/>
     </row>
-    <row r="50" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" s="18">
         <v>1</v>
       </c>
@@ -3611,7 +3611,7 @@
       <c r="X50" s="21"/>
       <c r="Y50" s="21"/>
     </row>
-    <row r="51" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" s="18">
         <v>4</v>
       </c>
@@ -3663,7 +3663,7 @@
       <c r="X51" s="21"/>
       <c r="Y51" s="21"/>
     </row>
-    <row r="52" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" s="18">
         <v>4</v>
       </c>
@@ -3713,7 +3713,7 @@
       <c r="X52" s="21"/>
       <c r="Y52" s="21"/>
     </row>
-    <row r="53" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" s="18">
         <v>3</v>
       </c>
@@ -3795,7 +3795,7 @@
       <c r="X54" s="21"/>
       <c r="Y54" s="21"/>
     </row>
-    <row r="55" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" s="18">
         <v>1</v>
       </c>
@@ -3847,7 +3847,7 @@
       <c r="X55" s="21"/>
       <c r="Y55" s="21"/>
     </row>
-    <row r="56" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" s="18">
         <v>1</v>
       </c>
@@ -3897,7 +3897,7 @@
       <c r="X56" s="21"/>
       <c r="Y56" s="21"/>
     </row>
-    <row r="57" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" s="18">
         <v>1</v>
       </c>
@@ -3947,7 +3947,7 @@
       <c r="X57" s="21"/>
       <c r="Y57" s="21"/>
     </row>
-    <row r="58" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" s="18">
         <v>4</v>
       </c>
@@ -3997,7 +3997,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" s="18">
         <v>1</v>
       </c>
@@ -4047,7 +4047,7 @@
       <c r="X59" s="21"/>
       <c r="Y59" s="21"/>
     </row>
-    <row r="60" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" s="18">
         <v>4</v>
       </c>
@@ -4097,7 +4097,7 @@
       </c>
       <c r="Y60" s="21"/>
     </row>
-    <row r="61" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" s="18">
         <v>4</v>
       </c>
@@ -4149,7 +4149,7 @@
       </c>
       <c r="Y61" s="21"/>
     </row>
-    <row r="62" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" s="18">
         <v>1</v>
       </c>
@@ -4199,7 +4199,7 @@
       <c r="X62" s="21"/>
       <c r="Y62" s="21"/>
     </row>
-    <row r="63" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" s="18">
         <v>4</v>
       </c>
@@ -4251,7 +4251,7 @@
       <c r="X63" s="21"/>
       <c r="Y63" s="21"/>
     </row>
-    <row r="64" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" s="18">
         <v>1</v>
       </c>
@@ -4301,7 +4301,7 @@
       <c r="X64" s="21"/>
       <c r="Y64" s="21"/>
     </row>
-    <row r="65" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" s="18">
         <v>4</v>
       </c>
@@ -4351,7 +4351,7 @@
       <c r="X65" s="21"/>
       <c r="Y65" s="21"/>
     </row>
-    <row r="66" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" s="18">
         <v>4</v>
       </c>
@@ -4401,7 +4401,7 @@
       <c r="X66" s="21"/>
       <c r="Y66" s="21"/>
     </row>
-    <row r="67" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" s="18">
         <v>1</v>
       </c>
@@ -4451,7 +4451,7 @@
       <c r="X67" s="21"/>
       <c r="Y67" s="21"/>
     </row>
-    <row r="68" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68" s="18">
         <v>1</v>
       </c>
@@ -4501,7 +4501,7 @@
       <c r="X68" s="21"/>
       <c r="Y68" s="21"/>
     </row>
-    <row r="69" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" s="18">
         <v>4</v>
       </c>
@@ -4551,7 +4551,7 @@
       <c r="X69" s="21"/>
       <c r="Y69" s="21"/>
     </row>
-    <row r="70" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" s="18">
         <v>4</v>
       </c>
@@ -4599,7 +4599,7 @@
       <c r="X70" s="21"/>
       <c r="Y70" s="21"/>
     </row>
-    <row r="71" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71" s="18">
         <v>1</v>
       </c>
@@ -4653,7 +4653,7 @@
       <c r="X71" s="21"/>
       <c r="Y71" s="21"/>
     </row>
-    <row r="72" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72" s="18">
         <v>1</v>
       </c>
@@ -4703,7 +4703,7 @@
       <c r="X72" s="21"/>
       <c r="Y72" s="21"/>
     </row>
-    <row r="73" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73" s="18">
         <v>1</v>
       </c>
@@ -4755,7 +4755,7 @@
       <c r="X73" s="21"/>
       <c r="Y73" s="21"/>
     </row>
-    <row r="74" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74" s="18">
         <v>4</v>
       </c>
@@ -4805,7 +4805,7 @@
       <c r="X74" s="21"/>
       <c r="Y74" s="21"/>
     </row>
-    <row r="75" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75" s="18">
         <v>2</v>
       </c>
@@ -4855,7 +4855,7 @@
       <c r="X75" s="21"/>
       <c r="Y75" s="21"/>
     </row>
-    <row r="76" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" s="18">
         <v>2</v>
       </c>
@@ -4905,7 +4905,7 @@
       <c r="X76" s="21"/>
       <c r="Y76" s="21"/>
     </row>
-    <row r="77" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" s="18">
         <v>4</v>
       </c>
@@ -4955,7 +4955,7 @@
       <c r="X77" s="21"/>
       <c r="Y77" s="21"/>
     </row>
-    <row r="78" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" s="18">
         <v>2</v>
       </c>
@@ -5005,7 +5005,7 @@
       <c r="X78" s="21"/>
       <c r="Y78" s="21"/>
     </row>
-    <row r="79" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" s="18">
         <v>2</v>
       </c>
@@ -5055,7 +5055,7 @@
       <c r="X79" s="21"/>
       <c r="Y79" s="21"/>
     </row>
-    <row r="80" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" s="18">
         <v>3</v>
       </c>
@@ -5105,7 +5105,7 @@
       <c r="X80" s="21"/>
       <c r="Y80" s="21"/>
     </row>
-    <row r="81" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" s="18">
         <v>1</v>
       </c>
@@ -5187,7 +5187,7 @@
       <c r="X82" s="21"/>
       <c r="Y82" s="21"/>
     </row>
-    <row r="83" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83" s="18">
         <v>1</v>
       </c>
@@ -5237,7 +5237,7 @@
       <c r="X83" s="21"/>
       <c r="Y83" s="21"/>
     </row>
-    <row r="84" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84" s="18">
         <v>1</v>
       </c>
@@ -5289,7 +5289,7 @@
       <c r="X84" s="21"/>
       <c r="Y84" s="21"/>
     </row>
-    <row r="85" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85" s="18">
         <v>1</v>
       </c>
@@ -5339,7 +5339,7 @@
       <c r="X85" s="21"/>
       <c r="Y85" s="21"/>
     </row>
-    <row r="86" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86" s="18">
         <v>4</v>
       </c>
@@ -5387,7 +5387,7 @@
       <c r="X86" s="21"/>
       <c r="Y86" s="21"/>
     </row>
-    <row r="87" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87" s="18">
         <v>2</v>
       </c>
@@ -5437,7 +5437,7 @@
       <c r="X87" s="21"/>
       <c r="Y87" s="21"/>
     </row>
-    <row r="88" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88" s="18">
         <v>4</v>
       </c>
@@ -5487,7 +5487,7 @@
       <c r="X88" s="21"/>
       <c r="Y88" s="21"/>
     </row>
-    <row r="89" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89" s="18">
         <v>1</v>
       </c>
@@ -5537,7 +5537,7 @@
       <c r="X89" s="21"/>
       <c r="Y89" s="21"/>
     </row>
-    <row r="90" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90" s="18">
         <v>1</v>
       </c>
@@ -5587,7 +5587,7 @@
       <c r="X90" s="21"/>
       <c r="Y90" s="21"/>
     </row>
-    <row r="91" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91" s="18">
         <v>2</v>
       </c>
@@ -5637,7 +5637,7 @@
       <c r="X91" s="21"/>
       <c r="Y91" s="21"/>
     </row>
-    <row r="92" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92" s="18">
         <v>1</v>
       </c>
@@ -5687,7 +5687,7 @@
       <c r="X92" s="21"/>
       <c r="Y92" s="21"/>
     </row>
-    <row r="93" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A93" s="18">
         <v>1</v>
       </c>
@@ -5739,7 +5739,7 @@
       <c r="X93" s="21"/>
       <c r="Y93" s="21"/>
     </row>
-    <row r="94" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94" s="18">
         <v>3</v>
       </c>
@@ -5789,7 +5789,7 @@
       <c r="X94" s="21"/>
       <c r="Y94" s="21"/>
     </row>
-    <row r="95" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95" s="18">
         <v>2</v>
       </c>
@@ -5839,7 +5839,7 @@
       <c r="X95" s="21"/>
       <c r="Y95" s="21"/>
     </row>
-    <row r="96" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96" s="18">
         <v>4</v>
       </c>
@@ -5889,7 +5889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97" s="18">
         <v>2</v>
       </c>
@@ -5939,7 +5939,7 @@
       <c r="X97" s="21"/>
       <c r="Y97" s="21"/>
     </row>
-    <row r="98" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A98" s="18">
         <v>1</v>
       </c>
@@ -5989,7 +5989,7 @@
       <c r="X98" s="21"/>
       <c r="Y98" s="21"/>
     </row>
-    <row r="99" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A99" s="18">
         <v>1</v>
       </c>
@@ -6039,7 +6039,7 @@
       <c r="X99" s="21"/>
       <c r="Y99" s="21"/>
     </row>
-    <row r="100" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A100" s="18">
         <v>1</v>
       </c>
@@ -6089,7 +6089,7 @@
       <c r="X100" s="21"/>
       <c r="Y100" s="21"/>
     </row>
-    <row r="101" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A101" s="18">
         <v>1</v>
       </c>
@@ -6139,7 +6139,7 @@
       <c r="X101" s="21"/>
       <c r="Y101" s="21"/>
     </row>
-    <row r="102" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A102" s="18">
         <v>1</v>
       </c>
@@ -6189,7 +6189,7 @@
       <c r="X102" s="21"/>
       <c r="Y102" s="21"/>
     </row>
-    <row r="103" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A103" s="18">
         <v>3</v>
       </c>
@@ -6239,7 +6239,7 @@
       <c r="X103" s="21"/>
       <c r="Y103" s="21"/>
     </row>
-    <row r="104" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104" s="18">
         <v>3</v>
       </c>
@@ -6289,7 +6289,7 @@
       <c r="X104" s="21"/>
       <c r="Y104" s="21"/>
     </row>
-    <row r="105" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A105" s="18">
         <v>2</v>
       </c>
@@ -6339,7 +6339,7 @@
       <c r="X105" s="21"/>
       <c r="Y105" s="21"/>
     </row>
-    <row r="106" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A106" s="18">
         <v>1</v>
       </c>
@@ -6389,7 +6389,7 @@
       <c r="X106" s="21"/>
       <c r="Y106" s="21"/>
     </row>
-    <row r="107" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A107" s="18">
         <v>2</v>
       </c>
@@ -6441,7 +6441,7 @@
       </c>
       <c r="Y107" s="21"/>
     </row>
-    <row r="108" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A108" s="18">
         <v>4</v>
       </c>
@@ -6491,7 +6491,7 @@
         <v>-190</v>
       </c>
     </row>
-    <row r="109" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A109" s="18">
         <v>4</v>
       </c>
@@ -6541,7 +6541,7 @@
       <c r="X109" s="21"/>
       <c r="Y109" s="21"/>
     </row>
-    <row r="110" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A110" s="18">
         <v>2</v>
       </c>
@@ -6591,7 +6591,7 @@
       <c r="X110" s="21"/>
       <c r="Y110" s="21"/>
     </row>
-    <row r="111" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A111" s="18">
         <v>2</v>
       </c>
@@ -6643,7 +6643,7 @@
       <c r="X111" s="21"/>
       <c r="Y111" s="21"/>
     </row>
-    <row r="112" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A112" s="18">
         <v>4</v>
       </c>
@@ -6693,7 +6693,7 @@
       <c r="X112" s="21"/>
       <c r="Y112" s="21"/>
     </row>
-    <row r="113" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A113" s="18">
         <v>5</v>
       </c>
@@ -6743,7 +6743,7 @@
       <c r="X113" s="21"/>
       <c r="Y113" s="21"/>
     </row>
-    <row r="114" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A114" s="18">
         <v>4</v>
       </c>
@@ -6791,7 +6791,7 @@
       <c r="X114" s="21"/>
       <c r="Y114" s="21"/>
     </row>
-    <row r="115" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A115" s="18">
         <v>1</v>
       </c>
@@ -6841,7 +6841,7 @@
       <c r="X115" s="21"/>
       <c r="Y115" s="21"/>
     </row>
-    <row r="116" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A116" s="18">
         <v>2</v>
       </c>
@@ -6891,7 +6891,7 @@
       <c r="X116" s="21"/>
       <c r="Y116" s="21"/>
     </row>
-    <row r="117" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A117" s="18">
         <v>4</v>
       </c>
@@ -6941,7 +6941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A118" s="18">
         <v>1</v>
       </c>
@@ -6993,7 +6993,7 @@
       <c r="X118" s="21"/>
       <c r="Y118" s="21"/>
     </row>
-    <row r="119" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A119" s="18">
         <v>1</v>
       </c>
@@ -7043,7 +7043,7 @@
       <c r="X119" s="21"/>
       <c r="Y119" s="21"/>
     </row>
-    <row r="120" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A120" s="18">
         <v>3</v>
       </c>
@@ -7091,7 +7091,7 @@
       <c r="X120" s="21"/>
       <c r="Y120" s="21"/>
     </row>
-    <row r="121" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A121" s="18">
         <v>1</v>
       </c>
@@ -7177,7 +7177,7 @@
       <c r="X122" s="21"/>
       <c r="Y122" s="21"/>
     </row>
-    <row r="123" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A123" s="18">
         <v>2</v>
       </c>
@@ -7231,7 +7231,7 @@
       </c>
       <c r="Y123" s="21"/>
     </row>
-    <row r="124" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A124" s="18">
         <v>3</v>
       </c>
@@ -7281,7 +7281,7 @@
       <c r="X124" s="21"/>
       <c r="Y124" s="21"/>
     </row>
-    <row r="125" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A125" s="18">
         <v>3</v>
       </c>
@@ -7331,7 +7331,7 @@
       <c r="X125" s="21"/>
       <c r="Y125" s="21"/>
     </row>
-    <row r="126" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A126" s="18">
         <v>1</v>
       </c>
@@ -7381,7 +7381,7 @@
       <c r="X126" s="21"/>
       <c r="Y126" s="21"/>
     </row>
-    <row r="127" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A127" s="18">
         <v>1</v>
       </c>
@@ -7431,7 +7431,7 @@
       <c r="X127" s="21"/>
       <c r="Y127" s="21"/>
     </row>
-    <row r="128" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A128" s="18">
         <v>1</v>
       </c>
@@ -7479,7 +7479,7 @@
       <c r="X128" s="21"/>
       <c r="Y128" s="21"/>
     </row>
-    <row r="129" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A129" s="18">
         <v>1</v>
       </c>
@@ -7529,7 +7529,7 @@
       <c r="X129" s="21"/>
       <c r="Y129" s="21"/>
     </row>
-    <row r="130" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A130" s="18">
         <v>2</v>
       </c>
@@ -7579,7 +7579,7 @@
       <c r="X130" s="21"/>
       <c r="Y130" s="21"/>
     </row>
-    <row r="131" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A131" s="18">
         <v>3</v>
       </c>
@@ -7629,7 +7629,7 @@
       <c r="X131" s="21"/>
       <c r="Y131" s="21"/>
     </row>
-    <row r="132" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A132" s="18">
         <v>1</v>
       </c>
@@ -7683,7 +7683,7 @@
       <c r="X132" s="21"/>
       <c r="Y132" s="21"/>
     </row>
-    <row r="133" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A133" s="18">
         <v>2</v>
       </c>
@@ -7779,7 +7779,7 @@
       <c r="X134" s="21"/>
       <c r="Y134" s="21"/>
     </row>
-    <row r="135" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A135" s="18">
         <v>2</v>
       </c>
@@ -7831,7 +7831,7 @@
       <c r="X135" s="21"/>
       <c r="Y135" s="21"/>
     </row>
-    <row r="136" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A136" s="18">
         <v>3</v>
       </c>
@@ -7881,7 +7881,7 @@
       <c r="X136" s="21"/>
       <c r="Y136" s="21"/>
     </row>
-    <row r="137" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A137" s="18">
         <v>2</v>
       </c>
@@ -7931,7 +7931,7 @@
       <c r="X137" s="21"/>
       <c r="Y137" s="21"/>
     </row>
-    <row r="138" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A138" s="18">
         <v>1</v>
       </c>
@@ -7981,7 +7981,7 @@
       <c r="X138" s="21"/>
       <c r="Y138" s="21"/>
     </row>
-    <row r="139" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A139" s="18">
         <v>1</v>
       </c>
@@ -8031,7 +8031,7 @@
       <c r="X139" s="21"/>
       <c r="Y139" s="21"/>
     </row>
-    <row r="140" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A140" s="18">
         <v>3</v>
       </c>
@@ -8081,7 +8081,7 @@
       <c r="X140" s="21"/>
       <c r="Y140" s="21"/>
     </row>
-    <row r="141" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A141" s="18">
         <v>1</v>
       </c>
@@ -8131,7 +8131,7 @@
       <c r="X141" s="21"/>
       <c r="Y141" s="21"/>
     </row>
-    <row r="142" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A142" s="18">
         <v>2</v>
       </c>
@@ -8181,7 +8181,7 @@
       <c r="X142" s="21"/>
       <c r="Y142" s="21"/>
     </row>
-    <row r="143" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A143" s="18">
         <v>1</v>
       </c>
@@ -8231,7 +8231,7 @@
       <c r="X143" s="21"/>
       <c r="Y143" s="21"/>
     </row>
-    <row r="144" spans="1:25" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A144" s="18">
         <v>2</v>
       </c>
@@ -8281,7 +8281,7 @@
       <c r="X144" s="21"/>
       <c r="Y144" s="21"/>
     </row>
-    <row r="145" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A145" s="18">
         <v>1</v>
       </c>
@@ -8333,7 +8333,7 @@
       <c r="X145" s="21"/>
       <c r="Y145" s="21"/>
     </row>
-    <row r="146" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A146" s="18">
         <v>3</v>
       </c>
@@ -8385,7 +8385,7 @@
       </c>
       <c r="Y146" s="21"/>
     </row>
-    <row r="147" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A147" s="18">
         <v>2</v>
       </c>
@@ -8435,7 +8435,7 @@
       <c r="X147" s="21"/>
       <c r="Y147" s="21"/>
     </row>
-    <row r="148" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A148" s="18">
         <v>1</v>
       </c>
@@ -8827,7 +8827,7 @@
       <c r="X155" s="21"/>
       <c r="Y155" s="21"/>
     </row>
-    <row r="156" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A156" s="18">
         <v>2</v>
       </c>
@@ -8913,7 +8913,7 @@
       <c r="X157" s="21"/>
       <c r="Y157" s="21"/>
     </row>
-    <row r="158" spans="1:25" s="23" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:25" s="23" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A158" s="18">
         <v>1</v>
       </c>
@@ -9970,7 +9970,13 @@
       <c r="X187" s="4"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Y178" xr:uid="{00000000-0009-0000-0000-000009000000}"/>
+  <autoFilter ref="A1:Y178" xr:uid="{00000000-0009-0000-0000-000009000000}">
+    <filterColumn colId="5">
+      <filters blank="1">
+        <dateGroupItem year="2020" month="3" day="20" dateTimeGrouping="day"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <mergeCells count="12">
     <mergeCell ref="G162:H162"/>
     <mergeCell ref="G165:H165"/>

</xml_diff>